<commit_message>
Analyse du Job Shop avec le solveur Evolutionnary
</commit_message>
<xml_diff>
--- a/26. Recherche opérationnelle en Excel/33 - MULTIPLES - JOB SHOP ET VOYAGEUR DE COMMERCE/Deal-with-Sequencing-Problems-using-Excel-Solver.xlsx
+++ b/26. Recherche opérationnelle en Excel/33 - MULTIPLES - JOB SHOP ET VOYAGEUR DE COMMERCE/Deal-with-Sequencing-Problems-using-Excel-Solver.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Recherche opérationnelle en Excel\33 - MULTIPLES - JOB SHOP ET VOYAGEUR DE COMMERCE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Index Function" sheetId="3" r:id="rId1"/>
@@ -71,9 +76,9 @@
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">11</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">6</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">AllDifferent</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">AllDifferent</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">"AllDifferent"</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">integer</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">integer</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">"integer"</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">1</definedName>
@@ -99,12 +104,12 @@
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Boston</t>
   </si>
@@ -201,17 +206,62 @@
   <si>
     <t>"=INDEX($C$3:$G$6,1,2)"</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Les variables de décision</t>
+  </si>
+  <si>
+    <t>La durée totale qu'on veut minimiser (function objectif)</t>
+  </si>
+  <si>
+    <t>Le job doit être fini le 32 ème jour par exemple</t>
+  </si>
+  <si>
+    <t>Durée d'un job</t>
+  </si>
+  <si>
+    <t>machine 1</t>
+  </si>
+  <si>
+    <t>Solveur result</t>
+  </si>
+  <si>
+    <t>JOB 2</t>
+  </si>
+  <si>
+    <t>JOB 3</t>
+  </si>
+  <si>
+    <t>JOB 1</t>
+  </si>
+  <si>
+    <t>machine 2</t>
+  </si>
+  <si>
+    <t>JOB 4</t>
+  </si>
+  <si>
+    <t>JOB 6</t>
+  </si>
+  <si>
+    <t>JOB 5</t>
+  </si>
+  <si>
+    <t>JOB SHOP !!!</t>
+  </si>
+  <si>
+    <t>Note : On voit que le solveur dispatche les jobs (tâches) sur les machines , en tenant compte de la date maximum de délivrance du job , et qu'il arrive à minimiser la date totale du projet !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -219,24 +269,78 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -407,10 +511,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -418,7 +521,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -465,9 +567,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,12 +597,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -522,7 +647,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,9 +679,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,6 +714,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -763,178 +890,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="8" max="8" width="9.125" style="5"/>
-    <col min="9" max="9" width="10.625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.625" style="5" customWidth="1"/>
-    <col min="11" max="14" width="9.125" style="5"/>
+    <col min="8" max="8" width="9.109375" style="4"/>
+    <col min="9" max="9" width="10.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="4" customWidth="1"/>
+    <col min="11" max="14" width="9.109375" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>983</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>1815</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>1991</v>
       </c>
       <c r="I3" s="1">
         <f>INDEX($C$3:$G$6,1,2)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>983</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1205</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>1050</v>
       </c>
-      <c r="I4" s="4" t="str">
+      <c r="I4" s="3" t="str">
         <f>INDEX($C$3:$G$6,2,1)</f>
         <v>Chicago</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1815</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1205</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>801</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f>INDEX($C$3:$G$6,2,5)</f>
         <v>1050</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>1991</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>1050</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>801</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <f>INDEX($C$3:$G$6,3,2)</f>
         <v>1815</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:14" s="5" customFormat="1">
-      <c r="C7" s="26"/>
-    </row>
-    <row r="8" spans="2:14" s="5" customFormat="1">
-      <c r="C8" s="26"/>
-    </row>
-    <row r="9" spans="2:14" s="5" customFormat="1">
-      <c r="C9" s="26"/>
-    </row>
-    <row r="10" spans="2:14" s="5" customFormat="1">
-      <c r="C10" s="26"/>
-    </row>
-    <row r="11" spans="2:14" s="5" customFormat="1">
-      <c r="C11" s="26"/>
-    </row>
-    <row r="12" spans="2:14" s="5" customFormat="1">
-      <c r="C12" s="26"/>
-    </row>
-    <row r="13" spans="2:14" s="5" customFormat="1">
-      <c r="C13" s="26"/>
+    <row r="7" spans="2:14" s="4" customFormat="1">
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="2:14" s="4" customFormat="1">
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="2:14" s="4" customFormat="1">
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="2:14" s="4" customFormat="1">
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="2:14" s="4" customFormat="1">
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="2:14" s="4" customFormat="1">
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="2:14" s="4" customFormat="1">
+      <c r="C13" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -944,650 +1071,650 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.125" customWidth="1"/>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="12" max="12" width="10.75" customWidth="1"/>
-    <col min="18" max="18" width="9.625" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:18">
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>983</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>1815</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>1991</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>3036</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>1539</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>213</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>2664</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>792</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>2385</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <v>2612</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="15">
         <v>10</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <f>INDEX($D$3:$N$13,$P13,$P3)</f>
         <v>817</v>
       </c>
-      <c r="R3" s="13" t="str">
+      <c r="R3" s="11" t="str">
         <f>VLOOKUP($P3,$B$3:$C$13,2,FALSE)</f>
         <v>SF</v>
       </c>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>983</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1205</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>1050</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>2112</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>1390</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>840</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>1729</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>457</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>2212</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>2052</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="16">
         <v>5</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="5">
         <f>INDEX($D$3:$N$13,$P3,$P4)</f>
         <v>403</v>
       </c>
-      <c r="R4" s="11" t="str">
+      <c r="R4" s="9" t="str">
         <f t="shared" ref="R4:R13" si="0">VLOOKUP($P4,$B$3:$C$13,2,FALSE)</f>
         <v>LA</v>
       </c>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1815</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1205</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>801</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>1425</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>1332</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>1604</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>1027</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>1237</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>1765</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>2404</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="16">
         <v>8</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <f t="shared" ref="Q5:Q13" si="1">INDEX($D$3:$N$13,$P4,$P5)</f>
         <v>398</v>
       </c>
-      <c r="R5" s="11" t="str">
+      <c r="R5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Phoenix</v>
       </c>
     </row>
     <row r="6" spans="2:18">
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1991</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1050</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>801</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>1174</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>1332</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>1780</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>836</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>1411</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>1765</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <v>1373</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="16">
         <v>3</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <f t="shared" si="1"/>
         <v>1027</v>
       </c>
-      <c r="R6" s="11" t="str">
+      <c r="R6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Dallas</v>
       </c>
     </row>
     <row r="7" spans="2:18">
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>3036</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>2112</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1425</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>1174</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>2757</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>2825</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>398</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>2456</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>403</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <v>1909</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="16">
         <v>6</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <f t="shared" si="1"/>
         <v>1332</v>
       </c>
-      <c r="R7" s="11" t="str">
+      <c r="R7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Miami</v>
       </c>
     </row>
     <row r="8" spans="2:18">
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>1539</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1390</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>1332</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>1332</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>2757</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>1258</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>2359</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>1250</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>3097</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <v>3389</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="16">
         <v>1</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <f t="shared" si="1"/>
         <v>1539</v>
       </c>
-      <c r="R8" s="11" t="str">
+      <c r="R8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Boston</v>
       </c>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>213</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>840</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>1604</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>1780</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>2825</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>1258</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>0</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <v>2442</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <v>386</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>3036</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>2900</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="16">
         <v>7</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-      <c r="R9" s="11" t="str">
+      <c r="R9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>NY</v>
       </c>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2664</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>1729</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>1027</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>836</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>398</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>2359</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>2442</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <v>2073</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>800</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="5">
         <v>1482</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="16">
         <v>9</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="5">
         <f t="shared" si="1"/>
         <v>386</v>
       </c>
-      <c r="R10" s="11" t="str">
+      <c r="R10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Pittsburgh</v>
       </c>
     </row>
     <row r="11" spans="2:18">
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>792</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>457</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>1237</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>1411</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>2456</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>1250</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>386</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>2073</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <v>0</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>2653</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="5">
         <v>2517</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="16">
         <v>2</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <f t="shared" si="1"/>
         <v>457</v>
       </c>
-      <c r="R11" s="11" t="str">
+      <c r="R11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Chicago</v>
       </c>
     </row>
     <row r="12" spans="2:18">
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <v>10</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>2385</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>2212</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>1765</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>1765</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>403</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>3097</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>3036</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="4">
         <v>800</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <v>2653</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <v>0</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="5">
         <v>817</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="16">
         <v>4</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="5">
         <f t="shared" si="1"/>
         <v>1050</v>
       </c>
-      <c r="R12" s="11" t="str">
+      <c r="R12" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Denver</v>
       </c>
     </row>
     <row r="13" spans="2:18">
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>2612</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>2052</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>2404</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>1373</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>1909</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>3389</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>2900</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>1482</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <v>2517</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="7">
         <v>817</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="8">
         <v>0</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="17">
         <v>11</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="8">
         <f t="shared" si="1"/>
         <v>1373</v>
       </c>
-      <c r="R13" s="12" t="str">
+      <c r="R13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Seattle</v>
       </c>
     </row>
     <row r="14" spans="2:18">
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q14" s="23">
+      <c r="Q14" s="21">
         <f>SUM(Q3:Q13)</f>
         <v>8995</v>
       </c>
@@ -1600,246 +1727,359 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="5.25" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="8.125" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="7.25" style="24" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="1:47">
+      <c r="A1" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47">
+      <c r="B2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="18">
+      <c r="M2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+    </row>
+    <row r="3" spans="1:47">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="42">
         <v>9</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="39">
         <v>32</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="13">
+      <c r="E3" s="4"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="35">
         <v>2</v>
       </c>
-      <c r="H3" s="2">
-        <f>VLOOKUP($G3,$B$3:$C$8,2,FALSE)</f>
+      <c r="H3" s="45">
+        <f t="shared" ref="H3:H8" si="0">VLOOKUP($G3,$B$3:$C$8,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <f>$H$3</f>
         <v>7</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="13">
-        <f>VLOOKUP($G3,$B$3:$D$8,3,FALSE)</f>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K8" si="1">VLOOKUP($G3,$B$3:$D$8,3,FALSE)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="18">
+      <c r="V3" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+    </row>
+    <row r="4" spans="1:47">
+      <c r="B4" s="16">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="42">
         <v>7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="39">
         <v>29</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="11">
+      <c r="E4" s="4"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="36">
         <v>3</v>
       </c>
-      <c r="H4" s="5">
-        <f>VLOOKUP($G4,$B$3:$C$8,2,FALSE)</f>
+      <c r="H4" s="42">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <f>SUM($H$3:$H4)</f>
         <v>15</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="11">
-        <f>VLOOKUP($G4,$B$3:$D$8,3,FALSE)</f>
+      <c r="K4" s="9">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="18">
+      <c r="AC4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="34"/>
+    </row>
+    <row r="5" spans="1:47">
+      <c r="B5" s="16">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="42">
         <v>8</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="39">
         <v>22</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="12">
-        <v>6</v>
-      </c>
-      <c r="H5" s="8">
-        <f>VLOOKUP($G5,$B$3:$C$8,2,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="E5" s="4"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="37">
+        <v>1</v>
+      </c>
+      <c r="H5" s="43">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I5" s="8">
         <f>SUM($H$3:$H5)</f>
+        <v>24</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="10">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47">
+      <c r="B6" s="16">
+        <v>4</v>
+      </c>
+      <c r="C6" s="42">
+        <v>18</v>
+      </c>
+      <c r="D6" s="39">
         <v>21</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="12">
-        <f>VLOOKUP($G5,$B$3:$D$8,3,FALSE)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="18">
+      <c r="E6" s="4"/>
+      <c r="F6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="35">
         <v>4</v>
       </c>
-      <c r="C6" s="5">
+      <c r="H6" s="42">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D6" s="6">
-        <v>21</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="13">
-        <v>4</v>
-      </c>
-      <c r="H6" s="5">
-        <f>VLOOKUP($G6,$B$3:$C$8,2,FALSE)</f>
-        <v>18</v>
-      </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <f>H$6</f>
         <v>18</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="11">
-        <f>VLOOKUP($G6,$B$3:$D$8,3,FALSE)</f>
+      <c r="K6" s="9">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="18">
+    <row r="7" spans="1:47">
+      <c r="B7" s="16">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="42">
         <v>9</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="39">
         <v>37</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5">
-        <f>VLOOKUP($G7,$B$3:$C$8,2,FALSE)</f>
+      <c r="E7" s="4"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="36">
+        <v>6</v>
+      </c>
+      <c r="H7" s="42">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="5">
+        <f>SUM($H$6:$H7)</f>
+        <v>24</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47">
+      <c r="B8" s="17">
+        <v>6</v>
+      </c>
+      <c r="C8" s="43">
+        <v>6</v>
+      </c>
+      <c r="D8" s="40">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="37">
+        <v>5</v>
+      </c>
+      <c r="H8" s="43">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I7" s="6">
-        <f>SUM($H$6:$H7)</f>
-        <v>27</v>
-      </c>
-      <c r="J7" s="24" t="s">
+      <c r="I8" s="8">
+        <f>SUM($H$6:$H8)</f>
+        <v>33</v>
+      </c>
+      <c r="J8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="11">
-        <f>VLOOKUP($G7,$B$3:$D$8,3,FALSE)</f>
+      <c r="K8" s="10">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47">
+      <c r="F9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="33">
+        <f>MAX(I5,I8)</f>
+        <v>33</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
+    </row>
+    <row r="10" spans="1:47">
+      <c r="AG10" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH10" s="51"/>
+      <c r="AI10" s="51"/>
+      <c r="AJ10" s="51"/>
+      <c r="AK10" s="51"/>
+      <c r="AL10" s="51"/>
+    </row>
+    <row r="11" spans="1:47">
+      <c r="F11" s="38"/>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM11" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN11" s="52"/>
+      <c r="AO11" s="52"/>
+      <c r="AP11" s="52"/>
+      <c r="AQ11" s="52"/>
+      <c r="AR11" s="52"/>
+      <c r="AS11" s="52"/>
+      <c r="AT11" s="52"/>
+      <c r="AU11" s="52"/>
+    </row>
+    <row r="12" spans="1:47">
+      <c r="F12" s="34"/>
+      <c r="G12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="19">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9">
-        <v>28</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="12">
-        <v>5</v>
-      </c>
-      <c r="H8" s="8">
-        <f>VLOOKUP($G8,$B$3:$C$8,2,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="I8" s="9">
-        <f>SUM($H$6:$H8)</f>
-        <v>36</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="12">
-        <f>VLOOKUP($G8,$B$3:$D$8,3,FALSE)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="F9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="10">
-        <f>MAX(I5,I8)</f>
-        <v>36</v>
+    <row r="13" spans="1:47">
+      <c r="F13" s="41"/>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47">
+      <c r="F14" s="44"/>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47">
+      <c r="F16" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>